<commit_message>
TEXT ANALYSIS - adding new media table
</commit_message>
<xml_diff>
--- a/FinalCorpus/mediaWords.xlsx
+++ b/FinalCorpus/mediaWords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\le_rap_francophone\Final Corpus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\le_rap_francophone\FinalCorpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDF3730-4AA1-4A77-98D7-87F191F3A71F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F826544-8E12-4A5E-ABD8-D6C772DACDD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6C5CF591-679C-41E9-B03E-168F6DCB78C1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="242">
   <si>
     <t>Social Media</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t xml:space="preserve">enregistrer </t>
+  </si>
+  <si>
+    <t>Chatter</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1187,7 @@
   <dimension ref="A1:R82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1466,7 +1469,7 @@
         <v>100</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>186</v>
+        <v>241</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>106</v>
@@ -1500,7 +1503,7 @@
         <v>95</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -1532,7 +1535,7 @@
         <v>96</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>107</v>
@@ -1562,7 +1565,7 @@
         <v>97</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>124</v>
@@ -1588,7 +1591,7 @@
         <v>98</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>138</v>
@@ -1614,7 +1617,7 @@
         <v>99</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>125</v>
@@ -1637,7 +1640,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>139</v>
@@ -1660,7 +1663,7 @@
         <v>58</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>140</v>
@@ -1683,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>141</v>
@@ -1706,7 +1709,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>142</v>
@@ -1728,8 +1731,8 @@
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
+      <c r="C16" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>143</v>
@@ -1746,7 +1749,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>126</v>
@@ -1763,7 +1766,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>144</v>
@@ -1780,7 +1783,7 @@
         <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>145</v>
@@ -1795,6 +1798,9 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>127</v>
@@ -2018,6 +2024,7 @@
       <c r="A57" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="C57"/>
       <c r="F57"/>
       <c r="I57"/>
       <c r="K57"/>
@@ -2034,6 +2041,7 @@
       <c r="A59" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="C59" s="5"/>
       <c r="O59" s="5"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.35">
@@ -2089,12 +2097,12 @@
         <v>83</v>
       </c>
       <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="C68" s="5"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
@@ -2134,6 +2142,7 @@
       <c r="O75"/>
     </row>
     <row r="76" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C76"/>
       <c r="F76"/>
       <c r="I76"/>
       <c r="K76"/>
@@ -2144,6 +2153,7 @@
       <c r="C77" s="5"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C78" s="5"/>
       <c r="O78" s="5"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>